<commit_message>
BEFORE - PUBLISH ALL
</commit_message>
<xml_diff>
--- a/LİNKLER_Ademden.xlsx
+++ b/LİNKLER_Ademden.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mADEMatik\Desktop\GEO12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04BD0DE3-3552-4339-99C6-589994CBEC0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED41F8F3-D6D7-461B-B073-BF8716BE33BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="77">
   <si>
     <t>DERS KİTAPLARINDA YER ALAN KAREKOD BİLGİLERİ</t>
   </si>
@@ -234,6 +234,51 @@
   </si>
   <si>
     <t>http://kitap.eba.gov.tr/KodSor.php?KOD=51889</t>
+  </si>
+  <si>
+    <t>fm_eksorular1_mk</t>
+  </si>
+  <si>
+    <t>fm_eksorular2_mk</t>
+  </si>
+  <si>
+    <t>fm_eksorular3_mk</t>
+  </si>
+  <si>
+    <t>fm_eksorular4_mk</t>
+  </si>
+  <si>
+    <t>fm_eksorular5_mk</t>
+  </si>
+  <si>
+    <t>http://kitap.eba.gov.tr/KodSor.php?KOD=51912</t>
+  </si>
+  <si>
+    <t>http://kitap.eba.gov.tr/KodSor.php?KOD=51911</t>
+  </si>
+  <si>
+    <t>http://kitap.eba.gov.tr/KodSor.php?KOD=51910</t>
+  </si>
+  <si>
+    <t>http://kitap.eba.gov.tr/KodSor.php?KOD=51909</t>
+  </si>
+  <si>
+    <t>http://kitap.eba.gov.tr/KodSor.php?KOD=51908</t>
+  </si>
+  <si>
+    <t>https://ders.eba.gov.tr/ders//redirectContent.jsp?resourceId=c8febc44e2b0823c9cb2e19d7e4a9278&amp;resourceType=1&amp;resourceLocation=2</t>
+  </si>
+  <si>
+    <t>https://ders.eba.gov.tr/ders//redirectContent.jsp?resourceId=95cc668f83f47573d46878f2e3e12b37&amp;resourceType=1&amp;resourceLocation=2</t>
+  </si>
+  <si>
+    <t>https://ders.eba.gov.tr/ders//redirectContent.jsp?resourceId=320a30576cde51b3b60e5fbb3ef804ca&amp;resourceType=1&amp;resourceLocation=2</t>
+  </si>
+  <si>
+    <t>https://ders.eba.gov.tr/ders//redirectContent.jsp?resourceId=9cd319a3b75b2868ea6536daa40f37bc&amp;resourceType=1&amp;resourceLocation=2</t>
+  </si>
+  <si>
+    <t>https://ders.eba.gov.tr/ders//redirectContent.jsp?resourceId=236a9b9767b383341efcb0bba4eaf4cf&amp;resourceType=1&amp;resourceLocation=2</t>
   </si>
 </sst>
 </file>
@@ -357,7 +402,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -418,6 +463,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Köprü" xfId="1" builtinId="8"/>
@@ -702,7 +748,7 @@
   <dimension ref="B2:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -710,7 +756,7 @@
     <col min="1" max="1" width="4.44140625" style="5" customWidth="1"/>
     <col min="2" max="2" width="8" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="118" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="8.77734375" style="5"/>
@@ -821,52 +867,82 @@
         <v>11</v>
       </c>
       <c r="C10" s="11"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="10"/>
+      <c r="D10" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="11"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
+      <c r="D11" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="11"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
+      <c r="D12" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="11"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
+      <c r="D13" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
+      <c r="D14" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
+      <c r="D15" s="15"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
     </row>

</xml_diff>